<commit_message>
add color theme: candy, psychedelic
</commit_message>
<xml_diff>
--- a/L_Table.xlsx
+++ b/L_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="780" windowWidth="35840" windowHeight="22700" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="920" yWindow="780" windowWidth="35840" windowHeight="22700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="10" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2526" uniqueCount="221">
   <si>
     <t>{</t>
     <phoneticPr fontId="1"/>
@@ -815,10 +815,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>G, W</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>G</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -863,10 +859,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>col_P</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>B</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -896,6 +888,66 @@
   </si>
   <si>
     <t>//</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G, Pi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>col_Candy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pi</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pi, Y, Ci</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pi, Y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R, G, B, Y, Pi, Pu, Ci, O</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>col_Psyche</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R, G, B</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>col_Pu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{ // Candy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{ // Psyche</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -943,7 +995,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1104,11 +1156,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1152,11 +1217,272 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="234">
+  <dxfs count="260">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4050,18 +4376,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="4" style="4" customWidth="1"/>
-    <col min="5" max="5" width="56.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="59.42578125" style="5" customWidth="1"/>
+    <col min="5" max="6" width="40.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
@@ -4069,14 +4394,16 @@
     <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="8.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" customWidth="1"/>
-    <col min="20" max="20" width="1.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.28515625" customWidth="1"/>
+    <col min="22" max="22" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="21" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:17" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="21" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:19" ht="22" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="16"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17" t="s">
@@ -4117,13 +4444,19 @@
         <v>178</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q2" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="S2" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="21" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -4170,13 +4503,19 @@
         <v>179</v>
       </c>
       <c r="P3" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q3" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="S3" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f>C4*2+D4*1+1</f>
         <v>1</v>
@@ -4215,7 +4554,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>186</v>
@@ -4224,13 +4563,19 @@
         <v>182</v>
       </c>
       <c r="P4" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q4" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <f t="shared" ref="A5:A7" si="0">C5*2+D5*1+1</f>
         <v>2</v>
@@ -4269,22 +4614,28 @@
         <v>3</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O5" s="7" t="s">
         <v>184</v>
       </c>
       <c r="P5" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q5" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="R5" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="S5" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4323,22 +4674,28 @@
         <v>3</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>183</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q6" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="R6" s="22" t="s">
+        <v>217</v>
+      </c>
+      <c r="S6" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4377,25 +4734,31 @@
         <v>3</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>187</v>
+        <v>206</v>
       </c>
       <c r="O7" s="7" t="s">
         <v>185</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q7" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="R7" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E3:F3 B1:D1048576">
-    <cfRule type="containsText" dxfId="233" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="259" priority="1" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4612,7 +4975,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H1:L2 H8:L8 I3:L7">
-    <cfRule type="containsText" dxfId="232" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="258" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4624,7 +4987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="81" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="81" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
@@ -5820,242 +6183,242 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="J1:L2 J12:L12 J57:L1048576">
-    <cfRule type="containsText" dxfId="231" priority="48" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="257" priority="48" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:L11 J3:L3">
-    <cfRule type="containsText" dxfId="230" priority="47" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="256" priority="47" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:L5">
-    <cfRule type="containsText" dxfId="229" priority="46" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="255" priority="46" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:L6">
-    <cfRule type="containsText" dxfId="228" priority="45" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="254" priority="45" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:L10">
-    <cfRule type="containsText" dxfId="227" priority="43" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="253" priority="43" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:L9">
-    <cfRule type="containsText" dxfId="226" priority="44" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="252" priority="44" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:L4">
-    <cfRule type="containsText" dxfId="225" priority="42" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="251" priority="42" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:L7">
-    <cfRule type="containsText" dxfId="224" priority="41" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="250" priority="41" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:L8">
-    <cfRule type="containsText" dxfId="223" priority="40" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="249" priority="40" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13:L13 J23:L23">
-    <cfRule type="containsText" dxfId="222" priority="39" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="248" priority="39" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:L22 J14:L14">
-    <cfRule type="containsText" dxfId="221" priority="38" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="247" priority="38" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:L16">
-    <cfRule type="containsText" dxfId="220" priority="37" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="246" priority="37" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:L17">
-    <cfRule type="containsText" dxfId="219" priority="36" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="245" priority="36" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="218" priority="34" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="244" priority="34" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:L20">
-    <cfRule type="containsText" dxfId="217" priority="35" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="243" priority="35" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J15:L15">
-    <cfRule type="containsText" dxfId="216" priority="33" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="242" priority="33" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:L18">
-    <cfRule type="containsText" dxfId="215" priority="32" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="241" priority="32" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:L19">
-    <cfRule type="containsText" dxfId="214" priority="31" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="240" priority="31" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:L24 J34:L34">
-    <cfRule type="containsText" dxfId="213" priority="30" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="239" priority="30" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:L33 J25:L25">
-    <cfRule type="containsText" dxfId="212" priority="29" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="238" priority="29" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:L27">
-    <cfRule type="containsText" dxfId="211" priority="28" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="237" priority="28" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:L28">
-    <cfRule type="containsText" dxfId="210" priority="27" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="236" priority="27" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:L32">
-    <cfRule type="containsText" dxfId="209" priority="25" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="235" priority="25" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:L31">
-    <cfRule type="containsText" dxfId="208" priority="26" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="234" priority="26" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26:L26">
-    <cfRule type="containsText" dxfId="207" priority="24" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="233" priority="24" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:L29">
-    <cfRule type="containsText" dxfId="206" priority="23" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="232" priority="23" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:L30">
-    <cfRule type="containsText" dxfId="205" priority="22" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="231" priority="22" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:L35 J45:L45">
-    <cfRule type="containsText" dxfId="204" priority="21" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="230" priority="21" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:L44 J36:L36">
-    <cfRule type="containsText" dxfId="203" priority="20" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="229" priority="20" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:L38">
-    <cfRule type="containsText" dxfId="202" priority="19" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="228" priority="19" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:L39">
-    <cfRule type="containsText" dxfId="201" priority="18" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="227" priority="18" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:L43">
-    <cfRule type="containsText" dxfId="200" priority="16" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="226" priority="16" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:L42">
-    <cfRule type="containsText" dxfId="199" priority="17" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="225" priority="17" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:L37">
-    <cfRule type="containsText" dxfId="198" priority="15" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="224" priority="15" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:L40">
-    <cfRule type="containsText" dxfId="197" priority="14" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="223" priority="14" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:L41">
-    <cfRule type="containsText" dxfId="196" priority="13" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="222" priority="13" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:L46 J56:L56">
-    <cfRule type="containsText" dxfId="195" priority="12" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="221" priority="12" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:L55 J47:L47">
-    <cfRule type="containsText" dxfId="194" priority="11" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="220" priority="11" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:L49">
-    <cfRule type="containsText" dxfId="193" priority="10" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="219" priority="10" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:L50">
-    <cfRule type="containsText" dxfId="192" priority="9" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="218" priority="9" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:L54">
-    <cfRule type="containsText" dxfId="191" priority="7" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="217" priority="7" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53:L53">
-    <cfRule type="containsText" dxfId="190" priority="8" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="216" priority="8" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:L48">
-    <cfRule type="containsText" dxfId="189" priority="6" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="215" priority="6" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:L51">
-    <cfRule type="containsText" dxfId="188" priority="5" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="214" priority="5" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:L52">
-    <cfRule type="containsText" dxfId="187" priority="4" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="213" priority="4" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24">
-    <cfRule type="containsText" dxfId="186" priority="3" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="212" priority="3" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
-    <cfRule type="containsText" dxfId="185" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="211" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46">
-    <cfRule type="containsText" dxfId="184" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="210" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J46)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8525,667 +8888,667 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="J1:L2 J13:L13 J147:L1048576">
-    <cfRule type="containsText" dxfId="183" priority="133" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="209" priority="133" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J12:L12 J4:L4">
-    <cfRule type="containsText" dxfId="182" priority="132" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="208" priority="132" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:L6">
-    <cfRule type="containsText" dxfId="181" priority="131" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="207" priority="131" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7:L7">
-    <cfRule type="containsText" dxfId="180" priority="130" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="206" priority="130" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:L11">
-    <cfRule type="containsText" dxfId="179" priority="128" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="205" priority="128" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:L10">
-    <cfRule type="containsText" dxfId="178" priority="129" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="204" priority="129" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:L5">
-    <cfRule type="containsText" dxfId="177" priority="127" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="203" priority="127" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8:L8">
-    <cfRule type="containsText" dxfId="176" priority="126" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="202" priority="126" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9:L9">
-    <cfRule type="containsText" dxfId="175" priority="125" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="201" priority="125" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:L14 J113:L113">
-    <cfRule type="containsText" dxfId="174" priority="124" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="200" priority="124" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J112:L112 J15:L15">
-    <cfRule type="containsText" dxfId="173" priority="123" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="199" priority="123" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:L17">
-    <cfRule type="containsText" dxfId="172" priority="122" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="198" priority="122" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18:L18">
-    <cfRule type="containsText" dxfId="171" priority="121" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="197" priority="121" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J23:L23">
-    <cfRule type="containsText" dxfId="170" priority="119" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="196" priority="119" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J22:L22">
-    <cfRule type="containsText" dxfId="169" priority="120" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="195" priority="120" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16:L16">
-    <cfRule type="containsText" dxfId="168" priority="118" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="194" priority="118" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J19:L19">
-    <cfRule type="containsText" dxfId="167" priority="117" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="193" priority="117" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20:L20">
-    <cfRule type="containsText" dxfId="166" priority="116" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="192" priority="116" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K114:L114 J124:L124">
-    <cfRule type="containsText" dxfId="165" priority="115" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="191" priority="115" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J123:L123 J115:L115">
-    <cfRule type="containsText" dxfId="164" priority="114" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="190" priority="114" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J117:L117">
-    <cfRule type="containsText" dxfId="163" priority="113" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="189" priority="113" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J118:L118">
-    <cfRule type="containsText" dxfId="162" priority="112" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="188" priority="112" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J122:L122">
-    <cfRule type="containsText" dxfId="161" priority="110" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="187" priority="110" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J121:L121">
-    <cfRule type="containsText" dxfId="160" priority="111" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="186" priority="111" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J121)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J116:L116">
-    <cfRule type="containsText" dxfId="159" priority="109" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="185" priority="109" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J116)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J119:L119">
-    <cfRule type="containsText" dxfId="158" priority="108" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="184" priority="108" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J120:L120">
-    <cfRule type="containsText" dxfId="157" priority="107" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="183" priority="107" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J120)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K125:L125 J135:L135">
-    <cfRule type="containsText" dxfId="156" priority="106" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="182" priority="106" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J134:L134 J126:L126">
-    <cfRule type="containsText" dxfId="155" priority="105" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="181" priority="105" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J128:L128">
-    <cfRule type="containsText" dxfId="154" priority="104" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="180" priority="104" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J128)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J129:L129">
-    <cfRule type="containsText" dxfId="153" priority="103" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="179" priority="103" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J129)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J133:L133">
-    <cfRule type="containsText" dxfId="152" priority="101" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="178" priority="101" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J133)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J132:L132">
-    <cfRule type="containsText" dxfId="151" priority="102" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="177" priority="102" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J127:L127">
-    <cfRule type="containsText" dxfId="150" priority="100" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="176" priority="100" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J127)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J130:L130">
-    <cfRule type="containsText" dxfId="149" priority="99" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="175" priority="99" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J130)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J131:L131">
-    <cfRule type="containsText" dxfId="148" priority="98" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="174" priority="98" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J131)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K136:L136 J146:L146">
-    <cfRule type="containsText" dxfId="147" priority="97" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="173" priority="97" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J145:L145 J137:L137">
-    <cfRule type="containsText" dxfId="146" priority="96" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="172" priority="96" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J137)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J139:L139">
-    <cfRule type="containsText" dxfId="145" priority="95" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="171" priority="95" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J139)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J140:L140">
-    <cfRule type="containsText" dxfId="144" priority="94" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="170" priority="94" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J144:L144">
-    <cfRule type="containsText" dxfId="143" priority="92" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="169" priority="92" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J143:L143">
-    <cfRule type="containsText" dxfId="142" priority="93" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="168" priority="93" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J143)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J138:L138">
-    <cfRule type="containsText" dxfId="141" priority="91" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="167" priority="91" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J138)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J141:L141">
-    <cfRule type="containsText" dxfId="140" priority="90" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="166" priority="90" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J142:L142">
-    <cfRule type="containsText" dxfId="139" priority="89" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="165" priority="89" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J114">
-    <cfRule type="containsText" dxfId="138" priority="88" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="164" priority="88" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J125">
-    <cfRule type="containsText" dxfId="137" priority="87" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="163" priority="87" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136">
-    <cfRule type="containsText" dxfId="136" priority="86" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="162" priority="86" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J136)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:L3">
-    <cfRule type="containsText" dxfId="135" priority="85" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="161" priority="85" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:L21">
-    <cfRule type="containsText" dxfId="134" priority="84" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="160" priority="84" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J24:L24 J35:L35">
-    <cfRule type="containsText" dxfId="133" priority="83" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="159" priority="83" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:L34 J26:L26">
-    <cfRule type="containsText" dxfId="132" priority="82" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="158" priority="82" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J28:L28">
-    <cfRule type="containsText" dxfId="131" priority="81" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="157" priority="81" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J29:L29">
-    <cfRule type="containsText" dxfId="130" priority="80" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="156" priority="80" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J33:L33">
-    <cfRule type="containsText" dxfId="129" priority="78" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="155" priority="78" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32:L32">
-    <cfRule type="containsText" dxfId="128" priority="79" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="154" priority="79" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:L27">
-    <cfRule type="containsText" dxfId="127" priority="77" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="153" priority="77" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J30:L30">
-    <cfRule type="containsText" dxfId="126" priority="76" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="152" priority="76" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J31:L31">
-    <cfRule type="containsText" dxfId="125" priority="75" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="151" priority="75" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:L36">
-    <cfRule type="containsText" dxfId="124" priority="74" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="150" priority="74" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:L37">
-    <cfRule type="containsText" dxfId="123" priority="73" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="149" priority="73" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J39:L39">
-    <cfRule type="containsText" dxfId="122" priority="72" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="148" priority="72" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:L40">
-    <cfRule type="containsText" dxfId="121" priority="71" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="147" priority="71" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:L45">
-    <cfRule type="containsText" dxfId="120" priority="69" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="146" priority="69" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:L44">
-    <cfRule type="containsText" dxfId="119" priority="70" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="145" priority="70" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38:L38">
-    <cfRule type="containsText" dxfId="118" priority="68" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="144" priority="68" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J41:L41">
-    <cfRule type="containsText" dxfId="117" priority="67" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="143" priority="67" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J42:L42">
-    <cfRule type="containsText" dxfId="116" priority="66" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="142" priority="66" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J25:L25">
-    <cfRule type="containsText" dxfId="115" priority="65" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="141" priority="65" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:L43">
-    <cfRule type="containsText" dxfId="114" priority="64" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="140" priority="64" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J57:L57">
-    <cfRule type="containsText" dxfId="113" priority="63" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="139" priority="63" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:L56 J48:L48">
-    <cfRule type="containsText" dxfId="112" priority="62" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="138" priority="62" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:L50">
-    <cfRule type="containsText" dxfId="111" priority="61" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="137" priority="61" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:L51">
-    <cfRule type="containsText" dxfId="110" priority="60" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="136" priority="60" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J55:L55">
-    <cfRule type="containsText" dxfId="109" priority="58" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="135" priority="58" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:L54">
-    <cfRule type="containsText" dxfId="108" priority="59" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="134" priority="59" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:L49">
-    <cfRule type="containsText" dxfId="107" priority="57" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="133" priority="57" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:L52">
-    <cfRule type="containsText" dxfId="106" priority="56" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="132" priority="56" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53:L53">
-    <cfRule type="containsText" dxfId="105" priority="55" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="131" priority="55" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J58:L58">
-    <cfRule type="containsText" dxfId="104" priority="54" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="130" priority="54" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J59:L59">
-    <cfRule type="containsText" dxfId="103" priority="53" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="129" priority="53" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J61:L61">
-    <cfRule type="containsText" dxfId="102" priority="52" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="128" priority="52" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62:L62">
-    <cfRule type="containsText" dxfId="101" priority="51" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="127" priority="51" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J67:L67">
-    <cfRule type="containsText" dxfId="100" priority="49" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="126" priority="49" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J66:L66">
-    <cfRule type="containsText" dxfId="99" priority="50" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="125" priority="50" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J66)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J60:L60">
-    <cfRule type="containsText" dxfId="98" priority="48" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="124" priority="48" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J63:L63">
-    <cfRule type="containsText" dxfId="97" priority="47" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="123" priority="47" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J64:L64">
-    <cfRule type="containsText" dxfId="96" priority="46" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="122" priority="46" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J47:L47">
-    <cfRule type="containsText" dxfId="95" priority="45" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="121" priority="45" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J65:L65">
-    <cfRule type="containsText" dxfId="94" priority="44" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="120" priority="44" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J79:L79">
-    <cfRule type="containsText" dxfId="93" priority="43" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="119" priority="43" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J79)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J78:L78 J70:L70">
-    <cfRule type="containsText" dxfId="92" priority="42" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="118" priority="42" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J72:L72">
-    <cfRule type="containsText" dxfId="91" priority="41" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="117" priority="41" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J73:L73">
-    <cfRule type="containsText" dxfId="90" priority="40" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="116" priority="40" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J77:L77">
-    <cfRule type="containsText" dxfId="89" priority="38" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="115" priority="38" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J76:L76">
-    <cfRule type="containsText" dxfId="88" priority="39" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="114" priority="39" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J71:L71">
-    <cfRule type="containsText" dxfId="87" priority="37" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="113" priority="37" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J74:L74">
-    <cfRule type="containsText" dxfId="86" priority="36" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="112" priority="36" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J74)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J75:L75">
-    <cfRule type="containsText" dxfId="85" priority="35" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="111" priority="35" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J75)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J80:L80">
-    <cfRule type="containsText" dxfId="84" priority="34" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="110" priority="34" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:L81">
-    <cfRule type="containsText" dxfId="83" priority="33" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="109" priority="33" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J83:L83">
-    <cfRule type="containsText" dxfId="82" priority="32" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="108" priority="32" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J84:L84">
-    <cfRule type="containsText" dxfId="81" priority="31" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="107" priority="31" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J84)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J89:L89">
-    <cfRule type="containsText" dxfId="80" priority="29" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="106" priority="29" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J89)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J88:L88">
-    <cfRule type="containsText" dxfId="79" priority="30" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="105" priority="30" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J88)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J82:L82">
-    <cfRule type="containsText" dxfId="78" priority="28" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="104" priority="28" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J85:L85">
-    <cfRule type="containsText" dxfId="77" priority="27" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="103" priority="27" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J85)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J86:L86">
-    <cfRule type="containsText" dxfId="76" priority="26" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="102" priority="26" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J69:L69">
-    <cfRule type="containsText" dxfId="75" priority="25" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="101" priority="25" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J87:L87">
-    <cfRule type="containsText" dxfId="74" priority="24" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="100" priority="24" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J87)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J101:L101">
-    <cfRule type="containsText" dxfId="73" priority="23" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="99" priority="23" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J101)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J100:L100 J92:L92">
-    <cfRule type="containsText" dxfId="72" priority="22" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="98" priority="22" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J94:L94">
-    <cfRule type="containsText" dxfId="71" priority="21" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="97" priority="21" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J95:L95">
-    <cfRule type="containsText" dxfId="70" priority="20" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="96" priority="20" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J95)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J99:L99">
-    <cfRule type="containsText" dxfId="69" priority="18" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="95" priority="18" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J99)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J98:L98">
-    <cfRule type="containsText" dxfId="68" priority="19" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="94" priority="19" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J98)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J93:L93">
-    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J96:L96">
-    <cfRule type="containsText" dxfId="66" priority="16" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="92" priority="16" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J97:L97">
-    <cfRule type="containsText" dxfId="65" priority="15" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="91" priority="15" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J102:L102">
-    <cfRule type="containsText" dxfId="64" priority="14" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="90" priority="14" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J103:L103">
-    <cfRule type="containsText" dxfId="63" priority="13" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="89" priority="13" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J105:L105">
-    <cfRule type="containsText" dxfId="62" priority="12" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="88" priority="12" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J106:L106">
-    <cfRule type="containsText" dxfId="61" priority="11" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="87" priority="11" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J106)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J111:L111">
-    <cfRule type="containsText" dxfId="60" priority="9" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="86" priority="9" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J111)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J110:L110">
-    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="85" priority="10" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J104:L104">
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="84" priority="8" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J107:L107">
-    <cfRule type="containsText" dxfId="57" priority="7" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="83" priority="7" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J108:L108">
-    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="82" priority="6" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J91:L91">
-    <cfRule type="containsText" dxfId="55" priority="5" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="81" priority="5" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:L109">
-    <cfRule type="containsText" dxfId="54" priority="4" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="80" priority="4" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:L46">
-    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="79" priority="3" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:L68">
-    <cfRule type="containsText" dxfId="52" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="78" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J90:L90">
-    <cfRule type="containsText" dxfId="51" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",J90)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9481,12 +9844,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E1:I1 E7:I8 F2:I6 E16:I1048576 I9:I15">
-    <cfRule type="containsText" dxfId="50" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:H9 E15:H15 F10:H14">
-    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",E9)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9652,7 +10015,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B11">
         <v>1.5</v>
@@ -9800,22 +10163,22 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E1:I3 E4:F8 H4:J5 H6:H8 E13:F17 P1:T2 E9:I12 P10:T1048576 E18:I1048576">
-    <cfRule type="containsText" dxfId="48" priority="5" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="74" priority="5" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J8">
-    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:J14 H15:H17">
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="72" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J17">
-    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="71" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",I15)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9981,7 +10344,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -10129,27 +10492,27 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E1:F1048576 P1:T2 G12:I12 P10:T1048576 G18:I18">
-    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="70" priority="7" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:I3 G9:I11 H4:J5 H6:H8 G19:I1048576">
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="69" priority="5" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J8">
-    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:J14 H15:H17">
-    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",H13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:J17">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",I15)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10308,7 +10671,7 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="E1:I1048576">
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10318,10 +10681,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF96"/>
+  <dimension ref="A1:AF152"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="87" workbookViewId="0">
-      <selection activeCell="AH29" sqref="AH29"/>
+    <sheetView topLeftCell="A68" zoomScale="87" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
@@ -10351,7 +10714,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AC1" t="s">
         <v>144</v>
@@ -10365,7 +10728,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -11296,12 +11659,12 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
@@ -12041,7 +12404,7 @@
         <v>1</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>34</v>
@@ -12164,12 +12527,12 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.3">
@@ -13100,12 +13463,12 @@
     </row>
     <row r="72" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="1:32" x14ac:dyDescent="0.3">
@@ -13971,206 +14334,2752 @@
         <v>167</v>
       </c>
     </row>
-    <row r="96" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC97" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE97" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF97" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="98" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>34</v>
+      </c>
+      <c r="F98" t="s">
+        <v>57</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98" t="s">
+        <v>1</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98" t="s">
+        <v>34</v>
+      </c>
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98" t="s">
+        <v>34</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98" t="s">
+        <v>58</v>
+      </c>
+      <c r="O98" t="s">
+        <v>57</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="s">
+        <v>1</v>
+      </c>
+      <c r="R98">
+        <v>0</v>
+      </c>
+      <c r="S98" t="s">
+        <v>34</v>
+      </c>
+      <c r="T98">
+        <v>0</v>
+      </c>
+      <c r="U98" t="s">
+        <v>34</v>
+      </c>
+      <c r="V98">
+        <v>0</v>
+      </c>
+      <c r="W98" t="s">
+        <v>58</v>
+      </c>
+      <c r="X98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C99" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K99" s="1">
+        <v>0</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M99" s="1">
+        <v>0</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P99" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R99" s="1">
+        <v>0</v>
+      </c>
+      <c r="S99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T99" s="1">
+        <v>0</v>
+      </c>
+      <c r="U99" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V99" s="1">
+        <v>0</v>
+      </c>
+      <c r="W99" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X99" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC101" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD101" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE101" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF101" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="102" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102" t="s">
+        <v>34</v>
+      </c>
+      <c r="F102" t="s">
+        <v>57</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+      <c r="H102" t="s">
+        <v>1</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102" t="s">
+        <v>34</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102" t="s">
+        <v>34</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102" t="s">
+        <v>58</v>
+      </c>
+      <c r="O102" t="s">
+        <v>57</v>
+      </c>
+      <c r="P102">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>1</v>
+      </c>
+      <c r="R102">
+        <v>0</v>
+      </c>
+      <c r="S102" t="s">
+        <v>34</v>
+      </c>
+      <c r="T102">
+        <v>0</v>
+      </c>
+      <c r="U102" t="s">
+        <v>34</v>
+      </c>
+      <c r="V102">
+        <v>0</v>
+      </c>
+      <c r="W102" t="s">
+        <v>58</v>
+      </c>
+      <c r="X102" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C103" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K103" s="1">
+        <v>0</v>
+      </c>
+      <c r="L103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M103" s="1">
+        <v>0</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P103" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R103" s="1">
+        <v>0</v>
+      </c>
+      <c r="S103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T103" s="1">
+        <v>0</v>
+      </c>
+      <c r="U103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V103" s="1">
+        <v>0</v>
+      </c>
+      <c r="W103" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X103" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC105" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD105" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE105" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF105" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106">
+        <v>6</v>
+      </c>
+      <c r="E106" t="s">
+        <v>34</v>
+      </c>
+      <c r="F106" t="s">
+        <v>57</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+      <c r="H106" t="s">
+        <v>1</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106" t="s">
+        <v>34</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106" t="s">
+        <v>34</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106" t="s">
+        <v>58</v>
+      </c>
+      <c r="O106" t="s">
+        <v>57</v>
+      </c>
+      <c r="P106">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>1</v>
+      </c>
+      <c r="R106">
+        <v>0</v>
+      </c>
+      <c r="S106" t="s">
+        <v>34</v>
+      </c>
+      <c r="T106">
+        <v>0</v>
+      </c>
+      <c r="U106" t="s">
+        <v>34</v>
+      </c>
+      <c r="V106">
+        <v>0</v>
+      </c>
+      <c r="W106" t="s">
+        <v>58</v>
+      </c>
+      <c r="X106" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+      <c r="E107" t="s">
+        <v>34</v>
+      </c>
+      <c r="F107" t="s">
+        <v>57</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107" t="s">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107" t="s">
+        <v>34</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107" t="s">
+        <v>34</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107" t="s">
+        <v>58</v>
+      </c>
+      <c r="O107" t="s">
+        <v>57</v>
+      </c>
+      <c r="P107">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>1</v>
+      </c>
+      <c r="R107">
+        <v>0</v>
+      </c>
+      <c r="S107" t="s">
+        <v>34</v>
+      </c>
+      <c r="T107">
+        <v>0</v>
+      </c>
+      <c r="U107" t="s">
+        <v>34</v>
+      </c>
+      <c r="V107">
+        <v>0</v>
+      </c>
+      <c r="W107" t="s">
+        <v>58</v>
+      </c>
+      <c r="X107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C108" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K108" s="1">
+        <v>0</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M108" s="1">
+        <v>0</v>
+      </c>
+      <c r="N108" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P108" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R108" s="1">
+        <v>0</v>
+      </c>
+      <c r="S108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T108" s="1">
+        <v>0</v>
+      </c>
+      <c r="U108" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V108" s="1">
+        <v>0</v>
+      </c>
+      <c r="W108" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X108" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC110" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD110" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE110" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF110" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111" t="s">
+        <v>34</v>
+      </c>
+      <c r="F111" t="s">
+        <v>57</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+      <c r="H111" t="s">
+        <v>1</v>
+      </c>
+      <c r="I111">
+        <v>0</v>
+      </c>
+      <c r="J111" t="s">
+        <v>34</v>
+      </c>
+      <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111" t="s">
+        <v>34</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111" t="s">
+        <v>58</v>
+      </c>
+      <c r="O111" t="s">
+        <v>57</v>
+      </c>
+      <c r="P111">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="s">
+        <v>1</v>
+      </c>
+      <c r="R111">
+        <v>0</v>
+      </c>
+      <c r="S111" t="s">
+        <v>34</v>
+      </c>
+      <c r="T111">
+        <v>0</v>
+      </c>
+      <c r="U111" t="s">
+        <v>34</v>
+      </c>
+      <c r="V111">
+        <v>0</v>
+      </c>
+      <c r="W111" t="s">
+        <v>58</v>
+      </c>
+      <c r="X111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G112" s="1">
+        <v>0</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K112" s="1">
+        <v>0</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M112" s="1">
+        <v>0</v>
+      </c>
+      <c r="N112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P112" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q112" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R112" s="1">
+        <v>0</v>
+      </c>
+      <c r="S112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T112" s="1">
+        <v>0</v>
+      </c>
+      <c r="U112" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V112" s="1">
+        <v>0</v>
+      </c>
+      <c r="W112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X112" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC114" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD114" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE114" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF114" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="115" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115">
+        <v>3</v>
+      </c>
+      <c r="E115" t="s">
+        <v>34</v>
+      </c>
+      <c r="F115" t="s">
+        <v>57</v>
+      </c>
+      <c r="G115">
+        <v>1</v>
+      </c>
+      <c r="H115" t="s">
+        <v>1</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115" t="s">
+        <v>34</v>
+      </c>
+      <c r="K115">
+        <v>1</v>
+      </c>
+      <c r="L115" t="s">
+        <v>34</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="N115" t="s">
+        <v>58</v>
+      </c>
+      <c r="O115" t="s">
+        <v>57</v>
+      </c>
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="s">
+        <v>1</v>
+      </c>
+      <c r="R115">
+        <v>0</v>
+      </c>
+      <c r="S115" t="s">
+        <v>34</v>
+      </c>
+      <c r="T115">
+        <v>0</v>
+      </c>
+      <c r="U115" t="s">
+        <v>34</v>
+      </c>
+      <c r="V115">
+        <v>0</v>
+      </c>
+      <c r="W115" t="s">
+        <v>58</v>
+      </c>
+      <c r="X115" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="116" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>34</v>
+      </c>
+      <c r="F116" t="s">
+        <v>57</v>
+      </c>
+      <c r="G116">
+        <v>1</v>
+      </c>
+      <c r="H116" t="s">
+        <v>1</v>
+      </c>
+      <c r="I116">
+        <v>1</v>
+      </c>
+      <c r="J116" t="s">
+        <v>34</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116" t="s">
+        <v>34</v>
+      </c>
+      <c r="M116">
+        <v>0</v>
+      </c>
+      <c r="N116" t="s">
+        <v>58</v>
+      </c>
+      <c r="O116" t="s">
+        <v>57</v>
+      </c>
+      <c r="P116">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>1</v>
+      </c>
+      <c r="R116">
+        <v>0</v>
+      </c>
+      <c r="S116" t="s">
+        <v>34</v>
+      </c>
+      <c r="T116">
+        <v>0</v>
+      </c>
+      <c r="U116" t="s">
+        <v>34</v>
+      </c>
+      <c r="V116">
+        <v>0</v>
+      </c>
+      <c r="W116" t="s">
+        <v>58</v>
+      </c>
+      <c r="X116" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117" t="s">
+        <v>34</v>
+      </c>
+      <c r="F117" t="s">
+        <v>57</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117" t="s">
+        <v>1</v>
+      </c>
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117" t="s">
+        <v>34</v>
+      </c>
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117" t="s">
+        <v>34</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117" t="s">
+        <v>58</v>
+      </c>
+      <c r="O117" t="s">
+        <v>57</v>
+      </c>
+      <c r="P117">
+        <v>0</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>1</v>
+      </c>
+      <c r="R117">
+        <v>0</v>
+      </c>
+      <c r="S117" t="s">
+        <v>34</v>
+      </c>
+      <c r="T117">
+        <v>0</v>
+      </c>
+      <c r="U117" t="s">
+        <v>34</v>
+      </c>
+      <c r="V117">
+        <v>0</v>
+      </c>
+      <c r="W117" t="s">
+        <v>58</v>
+      </c>
+      <c r="X117" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G118" s="1">
+        <v>0</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K118" s="1">
+        <v>0</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M118" s="1">
+        <v>0</v>
+      </c>
+      <c r="N118" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P118" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R118" s="1">
+        <v>0</v>
+      </c>
+      <c r="S118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T118" s="1">
+        <v>0</v>
+      </c>
+      <c r="U118" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V118" s="1">
+        <v>0</v>
+      </c>
+      <c r="W118" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X118" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="121" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="122" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC122" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD122" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE122" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF122" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="123" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C123" t="s">
+        <v>5</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123" t="s">
+        <v>34</v>
+      </c>
+      <c r="F123" t="s">
+        <v>57</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123" t="s">
+        <v>1</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123" t="s">
+        <v>34</v>
+      </c>
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123" t="s">
+        <v>34</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="N123" t="s">
+        <v>58</v>
+      </c>
+      <c r="O123" t="s">
+        <v>57</v>
+      </c>
+      <c r="P123">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>1</v>
+      </c>
+      <c r="R123">
+        <v>0</v>
+      </c>
+      <c r="S123" t="s">
+        <v>34</v>
+      </c>
+      <c r="T123">
+        <v>0</v>
+      </c>
+      <c r="U123" t="s">
+        <v>34</v>
+      </c>
+      <c r="V123">
+        <v>0</v>
+      </c>
+      <c r="W123" t="s">
+        <v>58</v>
+      </c>
+      <c r="X123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K124" s="1">
+        <v>0</v>
+      </c>
+      <c r="L124" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M124" s="1">
+        <v>0</v>
+      </c>
+      <c r="N124" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P124" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R124" s="1">
+        <v>0</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T124" s="1">
+        <v>0</v>
+      </c>
+      <c r="U124" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V124" s="1">
+        <v>0</v>
+      </c>
+      <c r="W124" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X124" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC126" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD126" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE126" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF126" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="127" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C127" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127" t="s">
+        <v>34</v>
+      </c>
+      <c r="F127" t="s">
+        <v>57</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127" t="s">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127" t="s">
+        <v>34</v>
+      </c>
+      <c r="K127">
+        <v>1</v>
+      </c>
+      <c r="L127" t="s">
+        <v>34</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127" t="s">
+        <v>58</v>
+      </c>
+      <c r="O127" t="s">
+        <v>57</v>
+      </c>
+      <c r="P127">
+        <v>0</v>
+      </c>
+      <c r="Q127" t="s">
+        <v>1</v>
+      </c>
+      <c r="R127">
+        <v>0</v>
+      </c>
+      <c r="S127" t="s">
+        <v>34</v>
+      </c>
+      <c r="T127">
+        <v>0</v>
+      </c>
+      <c r="U127" t="s">
+        <v>34</v>
+      </c>
+      <c r="V127">
+        <v>0</v>
+      </c>
+      <c r="W127" t="s">
+        <v>58</v>
+      </c>
+      <c r="X127" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="C128" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G128" s="1">
+        <v>0</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0</v>
+      </c>
+      <c r="J128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K128" s="1">
+        <v>0</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M128" s="1">
+        <v>0</v>
+      </c>
+      <c r="N128" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P128" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R128" s="1">
+        <v>0</v>
+      </c>
+      <c r="S128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T128" s="1">
+        <v>0</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V128" s="1">
+        <v>0</v>
+      </c>
+      <c r="W128" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X128" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC130" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD130" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE130" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF130" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="131" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C131" t="s">
+        <v>5</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131" t="s">
+        <v>34</v>
+      </c>
+      <c r="F131" t="s">
+        <v>57</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="H131" t="s">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131" t="s">
+        <v>34</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131" t="s">
+        <v>34</v>
+      </c>
+      <c r="M131">
+        <v>0</v>
+      </c>
+      <c r="N131" t="s">
+        <v>58</v>
+      </c>
+      <c r="O131" t="s">
+        <v>57</v>
+      </c>
+      <c r="P131">
+        <v>0</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>1</v>
+      </c>
+      <c r="R131">
+        <v>0</v>
+      </c>
+      <c r="S131" t="s">
+        <v>34</v>
+      </c>
+      <c r="T131">
+        <v>0</v>
+      </c>
+      <c r="U131" t="s">
+        <v>34</v>
+      </c>
+      <c r="V131">
+        <v>0</v>
+      </c>
+      <c r="W131" t="s">
+        <v>58</v>
+      </c>
+      <c r="X131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132" t="s">
+        <v>34</v>
+      </c>
+      <c r="F132" t="s">
+        <v>57</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
+      <c r="H132" t="s">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+      <c r="J132" t="s">
+        <v>34</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132" t="s">
+        <v>34</v>
+      </c>
+      <c r="M132">
+        <v>0</v>
+      </c>
+      <c r="N132" t="s">
+        <v>58</v>
+      </c>
+      <c r="O132" t="s">
+        <v>57</v>
+      </c>
+      <c r="P132">
+        <v>0</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>1</v>
+      </c>
+      <c r="R132">
+        <v>0</v>
+      </c>
+      <c r="S132" t="s">
+        <v>34</v>
+      </c>
+      <c r="T132">
+        <v>0</v>
+      </c>
+      <c r="U132" t="s">
+        <v>34</v>
+      </c>
+      <c r="V132">
+        <v>0</v>
+      </c>
+      <c r="W132" t="s">
+        <v>58</v>
+      </c>
+      <c r="X132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133" t="s">
+        <v>34</v>
+      </c>
+      <c r="F133" t="s">
+        <v>57</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133" t="s">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133" t="s">
+        <v>34</v>
+      </c>
+      <c r="K133">
+        <v>1</v>
+      </c>
+      <c r="L133" t="s">
+        <v>34</v>
+      </c>
+      <c r="M133">
+        <v>0</v>
+      </c>
+      <c r="N133" t="s">
+        <v>58</v>
+      </c>
+      <c r="O133" t="s">
+        <v>57</v>
+      </c>
+      <c r="P133">
+        <v>0</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>1</v>
+      </c>
+      <c r="R133">
+        <v>0</v>
+      </c>
+      <c r="S133" t="s">
+        <v>34</v>
+      </c>
+      <c r="T133">
+        <v>0</v>
+      </c>
+      <c r="U133" t="s">
+        <v>34</v>
+      </c>
+      <c r="V133">
+        <v>0</v>
+      </c>
+      <c r="W133" t="s">
+        <v>58</v>
+      </c>
+      <c r="X133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C134" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G134" s="1">
+        <v>0</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0</v>
+      </c>
+      <c r="J134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K134" s="1">
+        <v>0</v>
+      </c>
+      <c r="L134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M134" s="1">
+        <v>0</v>
+      </c>
+      <c r="N134" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P134" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R134" s="1">
+        <v>0</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T134" s="1">
+        <v>0</v>
+      </c>
+      <c r="U134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V134" s="1">
+        <v>0</v>
+      </c>
+      <c r="W134" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X134" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC136" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD136" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE136" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF136" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="137" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137" t="s">
+        <v>34</v>
+      </c>
+      <c r="F137" t="s">
+        <v>57</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+      <c r="H137" t="s">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+      <c r="J137" t="s">
+        <v>34</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137" t="s">
+        <v>34</v>
+      </c>
+      <c r="M137">
+        <v>0</v>
+      </c>
+      <c r="N137" t="s">
+        <v>58</v>
+      </c>
+      <c r="O137" t="s">
+        <v>57</v>
+      </c>
+      <c r="P137">
+        <v>0</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>1</v>
+      </c>
+      <c r="R137">
+        <v>0</v>
+      </c>
+      <c r="S137" t="s">
+        <v>34</v>
+      </c>
+      <c r="T137">
+        <v>0</v>
+      </c>
+      <c r="U137" t="s">
+        <v>34</v>
+      </c>
+      <c r="V137">
+        <v>0</v>
+      </c>
+      <c r="W137" t="s">
+        <v>58</v>
+      </c>
+      <c r="X137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D138" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+      <c r="H138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K138" s="1">
+        <v>0</v>
+      </c>
+      <c r="L138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M138" s="1">
+        <v>0</v>
+      </c>
+      <c r="N138" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P138" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R138" s="1">
+        <v>0</v>
+      </c>
+      <c r="S138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T138" s="1">
+        <v>0</v>
+      </c>
+      <c r="U138" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V138" s="1">
+        <v>0</v>
+      </c>
+      <c r="W138" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X138" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC140" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD140" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE140" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF140" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="141" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C141" t="s">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141" t="s">
+        <v>34</v>
+      </c>
+      <c r="F141" t="s">
+        <v>57</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141" t="s">
+        <v>34</v>
+      </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141" t="s">
+        <v>34</v>
+      </c>
+      <c r="M141">
+        <v>0</v>
+      </c>
+      <c r="N141" t="s">
+        <v>58</v>
+      </c>
+      <c r="O141" t="s">
+        <v>57</v>
+      </c>
+      <c r="P141">
+        <v>0</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>1</v>
+      </c>
+      <c r="R141">
+        <v>0</v>
+      </c>
+      <c r="S141" t="s">
+        <v>34</v>
+      </c>
+      <c r="T141">
+        <v>0</v>
+      </c>
+      <c r="U141" t="s">
+        <v>34</v>
+      </c>
+      <c r="V141">
+        <v>0</v>
+      </c>
+      <c r="W141" t="s">
+        <v>58</v>
+      </c>
+      <c r="X141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C142" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142" t="s">
+        <v>34</v>
+      </c>
+      <c r="F142" t="s">
+        <v>57</v>
+      </c>
+      <c r="G142">
+        <v>0</v>
+      </c>
+      <c r="H142" t="s">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+      <c r="J142" t="s">
+        <v>34</v>
+      </c>
+      <c r="K142">
+        <v>0</v>
+      </c>
+      <c r="L142" t="s">
+        <v>34</v>
+      </c>
+      <c r="M142">
+        <v>0</v>
+      </c>
+      <c r="N142" t="s">
+        <v>58</v>
+      </c>
+      <c r="O142" t="s">
+        <v>57</v>
+      </c>
+      <c r="P142">
+        <v>0</v>
+      </c>
+      <c r="Q142" t="s">
+        <v>1</v>
+      </c>
+      <c r="R142">
+        <v>0</v>
+      </c>
+      <c r="S142" t="s">
+        <v>34</v>
+      </c>
+      <c r="T142">
+        <v>0</v>
+      </c>
+      <c r="U142" t="s">
+        <v>34</v>
+      </c>
+      <c r="V142">
+        <v>0</v>
+      </c>
+      <c r="W142" t="s">
+        <v>58</v>
+      </c>
+      <c r="X142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C143" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
+        <v>34</v>
+      </c>
+      <c r="F143" t="s">
+        <v>57</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
+      <c r="H143" t="s">
+        <v>1</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143" t="s">
+        <v>34</v>
+      </c>
+      <c r="K143">
+        <v>1</v>
+      </c>
+      <c r="L143" t="s">
+        <v>34</v>
+      </c>
+      <c r="M143">
+        <v>0</v>
+      </c>
+      <c r="N143" t="s">
+        <v>58</v>
+      </c>
+      <c r="O143" t="s">
+        <v>57</v>
+      </c>
+      <c r="P143">
+        <v>0</v>
+      </c>
+      <c r="Q143" t="s">
+        <v>1</v>
+      </c>
+      <c r="R143">
+        <v>0</v>
+      </c>
+      <c r="S143" t="s">
+        <v>34</v>
+      </c>
+      <c r="T143">
+        <v>0</v>
+      </c>
+      <c r="U143" t="s">
+        <v>34</v>
+      </c>
+      <c r="V143">
+        <v>0</v>
+      </c>
+      <c r="W143" t="s">
+        <v>58</v>
+      </c>
+      <c r="X143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="C144" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144" t="s">
+        <v>34</v>
+      </c>
+      <c r="F144" t="s">
+        <v>57</v>
+      </c>
+      <c r="G144">
+        <v>1</v>
+      </c>
+      <c r="H144" t="s">
+        <v>1</v>
+      </c>
+      <c r="I144">
+        <v>1</v>
+      </c>
+      <c r="J144" t="s">
+        <v>34</v>
+      </c>
+      <c r="K144">
+        <v>0</v>
+      </c>
+      <c r="L144" t="s">
+        <v>34</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144" t="s">
+        <v>58</v>
+      </c>
+      <c r="O144" t="s">
+        <v>57</v>
+      </c>
+      <c r="P144">
+        <v>0</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>1</v>
+      </c>
+      <c r="R144">
+        <v>0</v>
+      </c>
+      <c r="S144" t="s">
+        <v>34</v>
+      </c>
+      <c r="T144">
+        <v>0</v>
+      </c>
+      <c r="U144" t="s">
+        <v>34</v>
+      </c>
+      <c r="V144">
+        <v>0</v>
+      </c>
+      <c r="W144" t="s">
+        <v>58</v>
+      </c>
+      <c r="X144" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C145" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145" t="s">
+        <v>34</v>
+      </c>
+      <c r="F145" t="s">
+        <v>57</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145" t="s">
+        <v>1</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145" t="s">
+        <v>34</v>
+      </c>
+      <c r="K145">
+        <v>1</v>
+      </c>
+      <c r="L145" t="s">
+        <v>34</v>
+      </c>
+      <c r="M145">
+        <v>0</v>
+      </c>
+      <c r="N145" t="s">
+        <v>58</v>
+      </c>
+      <c r="O145" t="s">
+        <v>57</v>
+      </c>
+      <c r="P145">
+        <v>0</v>
+      </c>
+      <c r="Q145" t="s">
+        <v>1</v>
+      </c>
+      <c r="R145">
+        <v>0</v>
+      </c>
+      <c r="S145" t="s">
+        <v>34</v>
+      </c>
+      <c r="T145">
+        <v>0</v>
+      </c>
+      <c r="U145" t="s">
+        <v>34</v>
+      </c>
+      <c r="V145">
+        <v>0</v>
+      </c>
+      <c r="W145" t="s">
+        <v>58</v>
+      </c>
+      <c r="X145" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C146" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>34</v>
+      </c>
+      <c r="F146" t="s">
+        <v>57</v>
+      </c>
+      <c r="G146">
+        <v>0.4</v>
+      </c>
+      <c r="H146" t="s">
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146" t="s">
+        <v>34</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146" t="s">
+        <v>34</v>
+      </c>
+      <c r="M146">
+        <v>0</v>
+      </c>
+      <c r="N146" t="s">
+        <v>58</v>
+      </c>
+      <c r="O146" t="s">
+        <v>57</v>
+      </c>
+      <c r="P146">
+        <v>0</v>
+      </c>
+      <c r="Q146" t="s">
+        <v>1</v>
+      </c>
+      <c r="R146">
+        <v>0</v>
+      </c>
+      <c r="S146" t="s">
+        <v>34</v>
+      </c>
+      <c r="T146">
+        <v>0</v>
+      </c>
+      <c r="U146" t="s">
+        <v>34</v>
+      </c>
+      <c r="V146">
+        <v>0</v>
+      </c>
+      <c r="W146" t="s">
+        <v>58</v>
+      </c>
+      <c r="X146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>34</v>
+      </c>
+      <c r="F147" t="s">
+        <v>57</v>
+      </c>
+      <c r="G147">
+        <v>0</v>
+      </c>
+      <c r="H147" t="s">
+        <v>1</v>
+      </c>
+      <c r="I147">
+        <v>1</v>
+      </c>
+      <c r="J147" t="s">
+        <v>34</v>
+      </c>
+      <c r="K147">
+        <v>1</v>
+      </c>
+      <c r="L147" t="s">
+        <v>34</v>
+      </c>
+      <c r="M147">
+        <v>0</v>
+      </c>
+      <c r="N147" t="s">
+        <v>58</v>
+      </c>
+      <c r="O147" t="s">
+        <v>57</v>
+      </c>
+      <c r="P147">
+        <v>0</v>
+      </c>
+      <c r="Q147" t="s">
+        <v>1</v>
+      </c>
+      <c r="R147">
+        <v>0</v>
+      </c>
+      <c r="S147" t="s">
+        <v>34</v>
+      </c>
+      <c r="T147">
+        <v>0</v>
+      </c>
+      <c r="U147" t="s">
+        <v>34</v>
+      </c>
+      <c r="V147">
+        <v>0</v>
+      </c>
+      <c r="W147" t="s">
+        <v>58</v>
+      </c>
+      <c r="X147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
+        <v>34</v>
+      </c>
+      <c r="F148" t="s">
+        <v>57</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+      <c r="H148" t="s">
+        <v>1</v>
+      </c>
+      <c r="I148">
+        <v>0.3</v>
+      </c>
+      <c r="J148" t="s">
+        <v>34</v>
+      </c>
+      <c r="K148">
+        <v>0</v>
+      </c>
+      <c r="L148" t="s">
+        <v>34</v>
+      </c>
+      <c r="M148">
+        <v>0</v>
+      </c>
+      <c r="N148" t="s">
+        <v>58</v>
+      </c>
+      <c r="O148" t="s">
+        <v>57</v>
+      </c>
+      <c r="P148">
+        <v>0</v>
+      </c>
+      <c r="Q148" t="s">
+        <v>1</v>
+      </c>
+      <c r="R148">
+        <v>0</v>
+      </c>
+      <c r="S148" t="s">
+        <v>34</v>
+      </c>
+      <c r="T148">
+        <v>0</v>
+      </c>
+      <c r="U148" t="s">
+        <v>34</v>
+      </c>
+      <c r="V148">
+        <v>0</v>
+      </c>
+      <c r="W148" t="s">
+        <v>58</v>
+      </c>
+      <c r="X148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="C149" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D149" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F149" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+      <c r="H149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I149" s="1">
+        <v>0</v>
+      </c>
+      <c r="J149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K149" s="1">
+        <v>0</v>
+      </c>
+      <c r="L149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M149" s="1">
+        <v>0</v>
+      </c>
+      <c r="N149" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P149" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q149" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R149" s="1">
+        <v>0</v>
+      </c>
+      <c r="S149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T149" s="1">
+        <v>0</v>
+      </c>
+      <c r="U149" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V149" s="1">
+        <v>0</v>
+      </c>
+      <c r="W149" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X149" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="152" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="AD3:AH6">
-    <cfRule type="containsText" dxfId="38" priority="210" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="64" priority="241" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD7:AH10">
-    <cfRule type="containsText" dxfId="37" priority="146" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="63" priority="177" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE11:AH11 AD12:AH14">
-    <cfRule type="containsText" dxfId="36" priority="145" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="62" priority="176" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE15:AH15 AD16:AH18">
-    <cfRule type="containsText" dxfId="35" priority="144" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="61" priority="175" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD20:AH20 AE19:AH19 AD23:AH25">
-    <cfRule type="containsText" dxfId="34" priority="143" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="60" priority="174" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD19">
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="59" priority="67" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD11">
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="58" priority="69" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD15">
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD43">
-    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD21:AH22">
-    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="55" priority="64" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD27:AH30">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="54" priority="63" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD31:AH34">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="53" priority="62" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE35:AH35 AD36:AH38">
-    <cfRule type="containsText" dxfId="26" priority="30" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="52" priority="61" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE39:AH39 AD40:AH42">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="51" priority="60" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD44:AH44 AE43:AH43 AD46:AH48">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="50" priority="59" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD67">
-    <cfRule type="containsText" dxfId="23" priority="16" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD35">
-    <cfRule type="containsText" dxfId="22" priority="27" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="48" priority="58" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD39">
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="47" priority="57" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD45:AH45">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="46" priority="55" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD68:AH68">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD50:AH53">
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="44" priority="54" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD54:AH57">
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="43" priority="53" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE58:AH58 AD59:AH59 AD61:AH62">
-    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="42" priority="52" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE63:AH63 AD64:AH66">
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="H">
+    <cfRule type="containsText" dxfId="41" priority="51" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH("H",AD63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE67:AH67 AD70:AH72">
+    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD58">
+    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD63">
+    <cfRule type="containsText" dxfId="38" priority="48" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD63)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD60:AH60">
+    <cfRule type="containsText" dxfId="37" priority="45" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD69:AH69">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD90">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD91:AH91">
+    <cfRule type="containsText" dxfId="34" priority="33" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD91)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD74:AH77">
+    <cfRule type="containsText" dxfId="33" priority="42" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD74)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD78:AH81">
+    <cfRule type="containsText" dxfId="32" priority="41" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE82:AH82 AD83:AH85">
+    <cfRule type="containsText" dxfId="31" priority="40" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE86:AH86 AD87:AH89">
+    <cfRule type="containsText" dxfId="30" priority="39" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE90:AH90 AD93:AH95">
+    <cfRule type="containsText" dxfId="29" priority="38" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD90)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD82">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD86">
+    <cfRule type="containsText" dxfId="27" priority="36" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD86)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD92:AH92">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD92)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD114">
+    <cfRule type="containsText" dxfId="25" priority="24" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD107:AH107">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD107)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD97:AH100">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD97)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD101:AH104">
+    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD101)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE105:AH105 AD106:AH106 AD108:AH109">
+    <cfRule type="containsText" dxfId="21" priority="29" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD105)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE110:AH110 AD111:AH113">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD110)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE114:AH114 AD118:AH120">
+    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD114)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD105">
+    <cfRule type="containsText" dxfId="18" priority="26" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD105)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD110">
+    <cfRule type="containsText" dxfId="17" priority="25" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD110)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD115:AH115">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD115)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD133:AH133">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD133)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD116:AH116">
     <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD67)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD58">
-    <cfRule type="containsText" dxfId="13" priority="18" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD63">
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD63)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD60:AH60">
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD69:AH69">
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD69)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD90">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD91:AH91">
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD91)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD74:AH77">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD74)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD78:AH81">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD78)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE82:AH82 AD83:AH85">
-    <cfRule type="containsText" dxfId="5" priority="9" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE86:AH86 AD87:AH89">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD86)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE90:AH90 AD93:AH95">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD90)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD82">
-    <cfRule type="containsText" dxfId="2" priority="6" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD82)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD86">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD86)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD92:AH92">
+      <formula>NOT(ISERROR(SEARCH("H",AD116)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD141:AH141">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD141)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD117:AH117">
+    <cfRule type="containsText" dxfId="12" priority="18" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD117)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD140">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD140)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD132:AH132">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD132)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD122:AH125">
+    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD122)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD126:AH129">
+    <cfRule type="containsText" dxfId="8" priority="16" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE130:AH130 AD131:AH131 AD134:AH135">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE136:AH136 AD137:AH139">
+    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD136)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE140:AH140 AD149:AH151">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD140)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD130">
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD136">
+    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD136)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD142:AH142">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD142)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD143:AH143">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="H">
+      <formula>NOT(ISERROR(SEARCH("H",AD143)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD144:AH148">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="H">
-      <formula>NOT(ISERROR(SEARCH("H",AD92)))</formula>
+      <formula>NOT(ISERROR(SEARCH("H",AD144)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implemented NumLogicalChs_Extended for more Randomness in Strobe animation
</commit_message>
<xml_diff>
--- a/L_Table.xlsx
+++ b/L_Table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="780" windowWidth="35840" windowHeight="22700" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="780" windowWidth="35840" windowHeight="22700" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Score" sheetId="10" r:id="rId1"/>
@@ -4378,7 +4378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+    <sheetView zoomScale="87" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -9861,8 +9861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J18"/>
   <sheetViews>
-    <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:J18"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>

</xml_diff>